<commit_message>
Se ajusto la interfaz de administración de las reservas
</commit_message>
<xml_diff>
--- a/webroot/reservas.xlsx
+++ b/webroot/reservas.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
   <si>
     <t>Reservas</t>
   </si>
@@ -23,7 +23,7 @@
     <t>Dia:</t>
   </si>
   <si>
-    <t>07/06/2021</t>
+    <t>19/03/2022</t>
   </si>
   <si>
     <t>Horario</t>
@@ -50,40 +50,46 @@
     <t>19:00:00</t>
   </si>
   <si>
+    <t>Rubén Miñarro</t>
+  </si>
+  <si>
+    <t>herrrubenminarro@gmail.com</t>
+  </si>
+  <si>
+    <t>Pendiente</t>
+  </si>
+  <si>
+    <t>Kart Adultos</t>
+  </si>
+  <si>
     <t>Vanneza Servín</t>
   </si>
   <si>
-    <t>0982355813</t>
-  </si>
-  <si>
     <t>vanezzaservin@gmail.com</t>
   </si>
   <si>
-    <t>Activo</t>
-  </si>
-  <si>
-    <t>Kart Adultos</t>
+    <t>19:15:00</t>
+  </si>
+  <si>
+    <t>Alberto Jose Suarez</t>
+  </si>
+  <si>
+    <t>0123654787</t>
+  </si>
+  <si>
+    <t>mail@mail.com</t>
   </si>
   <si>
     <t>19:30:00</t>
   </si>
   <si>
-    <t>Carlos Paez</t>
-  </si>
-  <si>
-    <t>098765431</t>
-  </si>
-  <si>
-    <t>mail@mail.com</t>
-  </si>
-  <si>
-    <t>20:00:00</t>
-  </si>
-  <si>
-    <t>Juan Pereza</t>
-  </si>
-  <si>
-    <t>0987412365</t>
+    <t>Juan Lopéz</t>
+  </si>
+  <si>
+    <t>test@test.com</t>
+  </si>
+  <si>
+    <t>Kart Niños</t>
   </si>
 </sst>
 </file>
@@ -790,17 +796,17 @@
       <c r="B6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="9">
+        <v>971975594</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="E6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="F6" s="10" t="s">
         <v>14</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>15</v>
       </c>
       <c r="G6" s="10">
         <v>3</v>
@@ -808,67 +814,95 @@
     </row>
     <row r="7" spans="1:7" customHeight="1" ht="17.9">
       <c r="A7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="13">
+        <v>982355813</v>
+      </c>
+      <c r="D7" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>19</v>
-      </c>
       <c r="E7" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="14" t="s">
-        <v>15</v>
-      </c>
       <c r="G7" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:7" customHeight="1" ht="17.9">
       <c r="A8" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="13">
+        <v>982355813</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" customHeight="1" ht="17.9">
+      <c r="A9" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="E9" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" customHeight="1" ht="17.9">
+      <c r="A10" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="B10" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" customHeight="1" ht="17.9">
-      <c r="A9" s="11"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-    </row>
-    <row r="10" spans="1:7" customHeight="1" ht="17.9">
-      <c r="A10" s="11"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
+      <c r="C10" s="13">
+        <v>56565656</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="14">
+        <v>4</v>
+      </c>
     </row>
     <row r="11" spans="1:7" customHeight="1" ht="17.9">
       <c r="A11" s="11"/>

</xml_diff>